<commit_message>
deleting and fixing files
</commit_message>
<xml_diff>
--- a/data/Pro_hooh_avgs.xlsx
+++ b/data/Pro_hooh_avgs.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkm/Documents/Talmy_research/Zinser_lab/Project_2_ROS_and_N/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dkm/Documents/Talmy_research/Zinser_lab/Projects/ROS_focused/Project_2_ROS_and_N/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE84B38B-2F0F-9244-843E-B40D8BCE0E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCBAA70-6D47-3B47-B0E5-E1492B265C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="520" windowWidth="27640" windowHeight="15900" xr2:uid="{B92FEC38-8B19-3F42-BBF5-045A5A2F8F47}"/>
+    <workbookView xWindow="800" yWindow="720" windowWidth="27640" windowHeight="15900" xr2:uid="{B92FEC38-8B19-3F42-BBF5-045A5A2F8F47}"/>
   </bookViews>
   <sheets>
     <sheet name="UH18301_vs_HOOH_avgs" sheetId="1" r:id="rId1"/>
     <sheet name="metadata_avgs" sheetId="2" r:id="rId2"/>
     <sheet name="raw data " sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="23">
   <si>
     <t>datatheif used to gather all points; have contacted Zinser for full counts</t>
   </si>
@@ -78,9 +78,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>avg</t>
-  </si>
-  <si>
     <t>flow</t>
   </si>
   <si>
@@ -90,9 +87,6 @@
     <t xml:space="preserve">time iin dayd </t>
   </si>
   <si>
-    <t xml:space="preserve">treatments in micromolar HOOH concentrations </t>
-  </si>
-  <si>
     <t xml:space="preserve">cell abundances in log scale already (plot is in !0^ format in publication ) </t>
   </si>
   <si>
@@ -103,6 +97,15 @@
   </si>
   <si>
     <t>negative tiimes at beginning of data sets changed to 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatmentsin nanoMolar HOOH concentrations </t>
+  </si>
+  <si>
+    <t>avg_log</t>
+  </si>
+  <si>
+    <t>avg_exp</t>
   </si>
 </sst>
 </file>
@@ -140,7 +143,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,21 +458,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05E5F671-28D5-C245-BF5E-F4489E725397}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -489,27 +492,30 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
@@ -523,25 +529,29 @@
       <c r="G2">
         <v>5.1111000000000004</v>
       </c>
-      <c r="H2" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="H2">
+        <f>10^G2</f>
+        <v>129151.66220708497</v>
+      </c>
+      <c r="I2" s="1">
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>6.2218999999999998</v>
+        <v>0.25924583333333334</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
@@ -555,25 +565,29 @@
       <c r="G3">
         <v>5.0461999999999998</v>
       </c>
-      <c r="H3" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
+      <c r="H3">
+        <f t="shared" ref="H3:H26" si="0">10^G3</f>
+        <v>111224.38165659865</v>
+      </c>
+      <c r="I3" s="1">
+        <v>50</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
-        <v>11.9962</v>
+        <v>0.49984166666666668</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -587,25 +601,29 @@
       <c r="G4">
         <v>5.1403999999999996</v>
       </c>
-      <c r="H4" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>138165.62311673295</v>
+      </c>
+      <c r="I4" s="1">
+        <v>50</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5">
-        <v>24.158000000000001</v>
+        <v>1.0065833333333334</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -619,25 +637,29 @@
       <c r="G5">
         <v>5.2538</v>
       </c>
-      <c r="H5" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I5" t="s">
-        <v>14</v>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>179390.73117342056</v>
+      </c>
+      <c r="I5" s="1">
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6">
-        <v>48.052700000000002</v>
+        <v>2.0021958333333334</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
@@ -651,25 +673,29 @@
       <c r="G6">
         <v>5.2187000000000001</v>
       </c>
-      <c r="H6" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>165462.65930505533</v>
+      </c>
+      <c r="I6" s="1">
+        <v>50</v>
       </c>
       <c r="J6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
@@ -683,25 +709,29 @@
       <c r="G7">
         <v>5.1111000000000004</v>
       </c>
-      <c r="H7" s="1">
-        <v>2</v>
-      </c>
-      <c r="I7" t="s">
-        <v>14</v>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>129151.66220708497</v>
+      </c>
+      <c r="I7" s="1">
+        <v>200</v>
       </c>
       <c r="J7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B8">
-        <v>6.2218999999999998</v>
+        <v>0.25924583333333334</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
@@ -715,25 +745,29 @@
       <c r="G8">
         <v>5.0461999999999998</v>
       </c>
-      <c r="H8" s="1">
-        <v>2</v>
-      </c>
-      <c r="I8" t="s">
-        <v>14</v>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>111224.38165659865</v>
+      </c>
+      <c r="I8" s="1">
+        <v>200</v>
       </c>
       <c r="J8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9">
-        <v>11.994400000000001</v>
+        <v>0.49976666666666669</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
@@ -747,25 +781,29 @@
       <c r="G9">
         <v>5.1123000000000003</v>
       </c>
-      <c r="H9" s="1">
-        <v>2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>14</v>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>129509.01491129331</v>
+      </c>
+      <c r="I9" s="1">
+        <v>200</v>
       </c>
       <c r="J9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>23.947099999999999</v>
+        <v>0.99779583333333333</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>11</v>
@@ -779,25 +817,29 @@
       <c r="G10">
         <v>5.1788999999999996</v>
       </c>
-      <c r="H10" s="1">
-        <v>2</v>
-      </c>
-      <c r="I10" t="s">
-        <v>14</v>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>150973.24853873104</v>
+      </c>
+      <c r="I10" s="1">
+        <v>200</v>
       </c>
       <c r="J10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B11">
-        <v>48.036999999999999</v>
+        <v>2.0015416666666668</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>11</v>
@@ -811,25 +853,29 @@
       <c r="G11">
         <v>4.9753999999999996</v>
       </c>
-      <c r="H11" s="1">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>14</v>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>94493.078903429952</v>
+      </c>
+      <c r="I11" s="1">
+        <v>200</v>
       </c>
       <c r="J11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D12" t="s">
         <v>11</v>
@@ -843,25 +889,29 @@
       <c r="G12">
         <v>5.1111000000000004</v>
       </c>
-      <c r="H12" s="1">
-        <v>4</v>
-      </c>
-      <c r="I12" t="s">
-        <v>14</v>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>129151.66220708497</v>
+      </c>
+      <c r="I12" s="1">
+        <v>400</v>
       </c>
       <c r="J12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13">
-        <v>6.2218999999999998</v>
+        <v>0.25924583333333334</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -875,25 +925,29 @@
       <c r="G13">
         <v>5.0461999999999998</v>
       </c>
-      <c r="H13" s="1">
-        <v>4</v>
-      </c>
-      <c r="I13" t="s">
-        <v>14</v>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>111224.38165659865</v>
+      </c>
+      <c r="I13" s="1">
+        <v>400</v>
       </c>
       <c r="J13" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B14">
-        <v>11.988300000000001</v>
+        <v>0.49951250000000003</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>11</v>
@@ -907,25 +961,29 @@
       <c r="G14">
         <v>5.0186999999999999</v>
       </c>
-      <c r="H14" s="1">
-        <v>4</v>
-      </c>
-      <c r="I14" t="s">
-        <v>14</v>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>104399.88012574866</v>
+      </c>
+      <c r="I14" s="1">
+        <v>400</v>
       </c>
       <c r="J14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>23.9344</v>
+        <v>0.99726666666666663</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -939,25 +997,29 @@
       <c r="G15">
         <v>4.9824000000000002</v>
       </c>
-      <c r="H15" s="1">
-        <v>4</v>
-      </c>
-      <c r="I15" t="s">
-        <v>14</v>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>96028.467920938318</v>
+      </c>
+      <c r="I15" s="1">
+        <v>400</v>
       </c>
       <c r="J15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B16">
-        <v>47.9696</v>
+        <v>1.9987333333333333</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D16" t="s">
         <v>11</v>
@@ -971,25 +1033,29 @@
       <c r="G16">
         <v>3.9275000000000002</v>
       </c>
-      <c r="H16" s="1">
-        <v>4</v>
-      </c>
-      <c r="I16" t="s">
-        <v>14</v>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>8462.5256880727065</v>
+      </c>
+      <c r="I16" s="1">
+        <v>400</v>
       </c>
       <c r="J16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
         <v>11</v>
@@ -1003,25 +1069,29 @@
       <c r="G17">
         <v>5.1111000000000004</v>
       </c>
-      <c r="H17" s="1">
-        <v>8</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>129151.66220708497</v>
+      </c>
+      <c r="I17" s="1">
+        <v>800</v>
       </c>
       <c r="J17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>6.0140000000000002</v>
+        <v>0.25058333333333332</v>
       </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -1035,25 +1105,29 @@
       <c r="G18">
         <v>5.0180999999999996</v>
       </c>
-      <c r="H18" s="1">
-        <v>8</v>
-      </c>
-      <c r="I18" t="s">
-        <v>14</v>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>104255.74594842384</v>
+      </c>
+      <c r="I18" s="1">
+        <v>800</v>
       </c>
       <c r="J18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>11.980499999999999</v>
+        <v>0.49918749999999995</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1067,25 +1141,29 @@
       <c r="G19">
         <v>4.8971</v>
       </c>
-      <c r="H19" s="1">
-        <v>8</v>
-      </c>
-      <c r="I19" t="s">
-        <v>14</v>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>78904.178028716866</v>
+      </c>
+      <c r="I19" s="1">
+        <v>800</v>
       </c>
       <c r="J19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>23.9146</v>
+        <v>0.99644166666666667</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
@@ -1099,25 +1177,29 @@
       <c r="G20">
         <v>4.6737000000000002</v>
       </c>
-      <c r="H20" s="1">
-        <v>8</v>
-      </c>
-      <c r="I20" t="s">
-        <v>14</v>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>47173.706426848839</v>
+      </c>
+      <c r="I20" s="1">
+        <v>800</v>
       </c>
       <c r="J20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21">
-        <v>47.920200000000001</v>
+        <v>1.996675</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D21" t="s">
         <v>11</v>
@@ -1131,25 +1213,29 @@
       <c r="G21">
         <v>3.1602000000000001</v>
       </c>
-      <c r="H21" s="1">
-        <v>8</v>
-      </c>
-      <c r="I21" t="s">
-        <v>14</v>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1446.1055736547355</v>
+      </c>
+      <c r="I21" s="1">
+        <v>800</v>
       </c>
       <c r="J21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1163,25 +1249,29 @@
       <c r="G22">
         <v>5.0549999999999997</v>
       </c>
-      <c r="H22" s="1">
-        <v>10</v>
-      </c>
-      <c r="I22" t="s">
-        <v>14</v>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>113501.08156723146</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1000</v>
       </c>
       <c r="J22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B23">
-        <v>5.9905999999999997</v>
+        <v>0.24960833333333332</v>
       </c>
       <c r="C23" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
         <v>11</v>
@@ -1195,25 +1285,29 @@
       <c r="G23">
         <v>4.6532</v>
       </c>
-      <c r="H23" s="1">
-        <v>10</v>
-      </c>
-      <c r="I23" t="s">
-        <v>14</v>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>44998.703387215079</v>
+      </c>
+      <c r="I23" s="1">
+        <v>1000</v>
       </c>
       <c r="J23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B24">
-        <v>12.1389</v>
+        <v>0.50578749999999995</v>
       </c>
       <c r="C24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
         <v>11</v>
@@ -1227,25 +1321,29 @@
       <c r="G24">
         <v>4.1578999999999997</v>
       </c>
-      <c r="H24" s="1">
-        <v>10</v>
-      </c>
-      <c r="I24" t="s">
-        <v>14</v>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>14384.673207789236</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1000</v>
       </c>
       <c r="J24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B25">
-        <v>24.056799999999999</v>
+        <v>1.0023666666666666</v>
       </c>
       <c r="C25" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D25" t="s">
         <v>11</v>
@@ -1259,25 +1357,29 @@
       <c r="G25">
         <v>3.6819000000000002</v>
       </c>
-      <c r="H25" s="1">
-        <v>10</v>
-      </c>
-      <c r="I25" t="s">
-        <v>14</v>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>4807.2864384397071</v>
+      </c>
+      <c r="I25" s="1">
+        <v>1000</v>
       </c>
       <c r="J25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B26">
-        <v>47.888300000000001</v>
+        <v>1.9953458333333334</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>11</v>
@@ -1291,14 +1393,18 @@
       <c r="G26">
         <v>2.6642999999999999</v>
       </c>
-      <c r="H26" s="1">
-        <v>10</v>
-      </c>
-      <c r="I26" t="s">
-        <v>14</v>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>461.63635154046779</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1000</v>
       </c>
       <c r="J26" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="K26" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1311,7 +1417,7 @@
   <dimension ref="B3:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,22 +1432,22 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>